<commit_message>
OUT OF TAT - UNDELIVERED TRACKON COURIER #CRM-3396
OUT OF TAT - UNDELIVERED TRACKON COURIER #CRM-3396
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/awb-shipment-pending.xlsx
+++ b/application/controllers/excel-templates/awb-shipment-pending.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="awb_number" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,11 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Awb No</t>
   </si>
   <si>
+    <t xml:space="preserve">Count</t>
+  </si>
+  <si>
     <t xml:space="preserve">Courier Name</t>
   </si>
   <si>
@@ -44,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">{spare:awb_no}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{spare:total_spare}</t>
   </si>
   <si>
     <t xml:space="preserve">{spare:courier_name}</t>
@@ -166,9 +172,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -208,119 +218,125 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X1000"/>
+  <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="0" width="26.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="37.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="23.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="25.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="24.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="22.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="20.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="25.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="26" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="12" style="0" width="26.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="37.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="23.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="25.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="24.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="22.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="20.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="25.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="G2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="5"/>
       <c r="J2" s="5"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>